<commit_message>
Backup QR Scanner data - 2025-10-29T04:19:32.699Z - Cache Bust: 1761711572699
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Immuno_hema_scanner1761641793286_8e9cc48f6e8793e4ce72349bce8e04df5ba55f2c8dbce18973fc024c02f4b8cf.xlsx
+++ b/log_history/Y4_B2526_Immuno_hema_scanner1761641793286_8e9cc48f6e8793e4ce72349bce8e04df5ba55f2c8dbce18973fc024c02f4b8cf.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -522,269 +522,9 @@
         <v>mai_elbadry@med.asu.edu.eg</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>221816</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C7" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D7" t="str">
-        <v>11:57:51</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>221872</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C8" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D8" t="str">
-        <v>11:58:14</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F8" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>221805</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C9" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D9" t="str">
-        <v>11:58:34</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F9" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>221880</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C10" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D10" t="str">
-        <v>11:58:41</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F10" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>221832</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C11" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D11" t="str">
-        <v>11:58:47</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F11" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>221767</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C12" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D12" t="str">
-        <v>11:58:53</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F12" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>221784</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C13" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D13" t="str">
-        <v>11:59:00</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F13" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>221781</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C14" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D14" t="str">
-        <v>11:59:06</v>
-      </c>
-      <c r="E14" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F14" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>221878</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C15" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D15" t="str">
-        <v>11:59:15</v>
-      </c>
-      <c r="E15" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F15" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>221797</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C16" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D16" t="str">
-        <v>11:59:46</v>
-      </c>
-      <c r="E16" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F16" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>221775</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C17" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D17" t="str">
-        <v>11:59:52</v>
-      </c>
-      <c r="E17" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F17" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>221853</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C18" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D18" t="str">
-        <v>12:00:12</v>
-      </c>
-      <c r="E18" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F18" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>221877</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Immuno&amp;hema</v>
-      </c>
-      <c r="C19" t="str">
-        <v>28/10/2025</v>
-      </c>
-      <c r="D19" t="str">
-        <v>12:00:22</v>
-      </c>
-      <c r="E19" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F19" t="str">
-        <v>mai_elbadry@med.asu.edu.eg</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>